<commit_message>
Refactor click.py logging messages for clarity; remove temporary Excel file
</commit_message>
<xml_diff>
--- a/data/list.xlsx
+++ b/data/list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\sellshit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D312C-8E6A-48B8-80DE-69796CF54FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8A039F-D9C4-4DCE-8873-CCA9CAE5B70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1006,12 +1006,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1041,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1083,6 +1089,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1303,14 +1322,15 @@
   </sheetPr>
   <dimension ref="A1:Y979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection sqref="A1:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="17.109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" style="5" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="5" customWidth="1"/>
@@ -1358,590 +1378,590 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+    <row r="2" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="21">
         <v>250</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="21">
         <v>175</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="19">
         <v>18614</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+    </row>
+    <row r="3" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="21">
         <v>100</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="21">
         <v>30</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="19">
         <v>18614</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+    </row>
+    <row r="4" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="21">
         <v>50</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="21">
         <v>30</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="19">
         <v>18614</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+    </row>
+    <row r="5" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
         <v>7</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="21">
         <v>30</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="21">
         <v>10</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="19">
         <v>18614</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+    </row>
+    <row r="6" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="21">
         <v>225</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="21">
         <v>175</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="19">
         <v>18614</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+    </row>
+    <row r="7" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="21">
         <v>75</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="21">
         <v>20</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="19">
         <v>18614</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+    </row>
+    <row r="8" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
         <v>13</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="21">
         <v>150</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="21">
         <v>80</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="19">
         <v>18614</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+    </row>
+    <row r="9" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
         <v>14</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="21">
         <v>45</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="21">
         <v>25</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="19">
         <v>18614</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+    </row>
+    <row r="10" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <v>16</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="21">
         <v>100</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="21">
         <v>30</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="19">
         <v>18614</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+    </row>
+    <row r="11" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>17</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="21">
         <v>50</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="21">
         <v>10</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="19">
         <v>18614</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+    </row>
+    <row r="12" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
         <v>18</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="21">
         <v>55</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="21">
         <v>10</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="19">
         <v>18614</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+    </row>
+    <row r="13" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
         <v>22</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="21">
         <v>40</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="21">
         <v>10</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="19">
         <v>18614</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+    </row>
+    <row r="14" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
         <v>24</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="21">
         <v>75</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="21">
         <v>5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="19">
         <v>18614</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
     </row>
     <row r="15" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
@@ -2573,50 +2593,50 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+    <row r="29" spans="1:25" s="23" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
         <v>45</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="21">
         <v>1100</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="21">
         <v>750</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="19">
         <v>18614</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">

</xml_diff>